<commit_message>
Update Operations.xlsx with electrical stuff V1
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -14,13 +14,13 @@
   <sheets>
     <sheet name="operations" sheetId="18" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
   <si>
     <t>Mobilisation</t>
   </si>
@@ -211,39 +211,9 @@
     <t>Seafast</t>
   </si>
   <si>
-    <t>Vessel positioning</t>
-  </si>
-  <si>
-    <t>Winch wire connection to cable pull-head</t>
-  </si>
-  <si>
-    <t>Cable float-out onto the beach zone</t>
-  </si>
-  <si>
-    <t>Cable layed into pre-excavated trench</t>
-  </si>
-  <si>
-    <t>Cable pull-in through HDD conduit to rig siite</t>
-  </si>
-  <si>
     <t>SeafloorEquipPrep</t>
   </si>
   <si>
-    <t>LF_VesPos</t>
-  </si>
-  <si>
-    <t>LF_PullHead</t>
-  </si>
-  <si>
-    <t>LF_FloatOut</t>
-  </si>
-  <si>
-    <t>LF_OCT</t>
-  </si>
-  <si>
-    <t>LF_HDD</t>
-  </si>
-  <si>
     <t>Vessels and Equipments Database</t>
   </si>
   <si>
@@ -305,6 +275,99 @@
   </si>
   <si>
     <t>Time: value [h]</t>
+  </si>
+  <si>
+    <t>LoadCableFactory</t>
+  </si>
+  <si>
+    <t>Loading cable from factory port</t>
+  </si>
+  <si>
+    <t>loadcable</t>
+  </si>
+  <si>
+    <t>Vessel Positioning + Connection to cable pull-head + Cable float-out + Cable lay into pre-excavated trench</t>
+  </si>
+  <si>
+    <t>Vessel positioning + Connection to cable pull-head + Cable float-out + Cable pull-in through HDD conduit</t>
+  </si>
+  <si>
+    <t>BurialToolDeploy</t>
+  </si>
+  <si>
+    <t>CableLayRoute</t>
+  </si>
+  <si>
+    <t>CableLayTrench</t>
+  </si>
+  <si>
+    <t>CableLayBurial</t>
+  </si>
+  <si>
+    <t>BurialToolRecov</t>
+  </si>
+  <si>
+    <t>CableLaySplitPipe</t>
+  </si>
+  <si>
+    <t>Recover cable burial tool</t>
+  </si>
+  <si>
+    <t>Deploy of Cable Burial Tool</t>
+  </si>
+  <si>
+    <t>Cable lay through cable route</t>
+  </si>
+  <si>
+    <t>Cable lay and burial through cable route</t>
+  </si>
+  <si>
+    <t>Cable lay through open trench</t>
+  </si>
+  <si>
+    <t>Cable lay with split pipes</t>
+  </si>
+  <si>
+    <t>H_progressrate</t>
+  </si>
+  <si>
+    <t>OnTerm_OCT</t>
+  </si>
+  <si>
+    <t>OnTerm_HDD</t>
+  </si>
+  <si>
+    <t>OffTerm_Dev_Con</t>
+  </si>
+  <si>
+    <t>OffTerm_DynCable</t>
+  </si>
+  <si>
+    <t>OffTerm_Dev_Jtube</t>
+  </si>
+  <si>
+    <t>OffTerm_CP_HardW</t>
+  </si>
+  <si>
+    <t>OffTerm_CP_Dry</t>
+  </si>
+  <si>
+    <t>OffTerm_CP_Wet</t>
+  </si>
+  <si>
+    <t>OffTerm_CP_Jtube</t>
+  </si>
+  <si>
+    <t>J-tube entrance inspection + Guide wire connection + Cable lay + Cable pull + Cable connection</t>
+  </si>
+  <si>
+    <t>Lower cable end to the seabed</t>
+  </si>
+  <si>
+    <t>Lower collection point to the seabed</t>
+  </si>
+  <si>
+    <t>Connect to guide wire + Lower cable and connection equip + Perform wet-mate connect + Recover connection equip</t>
   </si>
 </sst>
 </file>
@@ -356,7 +419,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -661,6 +724,50 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -687,12 +794,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -714,12 +815,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -762,12 +857,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -784,6 +873,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1090,16 +1197,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
@@ -1111,64 +1218,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>93</v>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="21">
         <v>100</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="26"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="23">
         <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1178,18 +1285,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="28"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="28"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="23">
         <v>102</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1199,18 +1306,18 @@
         <v>48</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="28"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="28"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="23">
         <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1218,20 +1325,20 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="28"/>
+        <v>66</v>
+      </c>
+      <c r="F5" s="24"/>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="28"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="23">
         <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1239,20 +1346,20 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="28"/>
+        <v>67</v>
+      </c>
+      <c r="F6" s="24"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="28"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="23">
         <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1260,20 +1367,20 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="28"/>
+        <v>68</v>
+      </c>
+      <c r="F7" s="24"/>
       <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="28"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="23">
         <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1281,20 +1388,20 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="29" t="s">
-        <v>74</v>
+      <c r="F8" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="28"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="27">
+        <v>63</v>
+      </c>
+      <c r="B9" s="23">
         <v>107</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1304,18 +1411,18 @@
         <v>1</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="28"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="28"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="23">
         <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1323,20 +1430,20 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="28"/>
+        <v>65</v>
+      </c>
+      <c r="F10" s="24"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="23">
         <v>109</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1346,614 +1453,845 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="28"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="26">
         <v>110</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>2</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="25">
+      <c r="E12" s="13"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="35">
         <v>200</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="16">
+      <c r="C13" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
+    </row>
+    <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="35">
+        <v>201</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="37">
+        <v>10</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="35">
+        <v>202</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="37">
+        <v>10</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39"/>
+    </row>
+    <row r="16" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="35">
+        <v>203</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="37">
+        <v>1</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+    </row>
+    <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="35">
+        <v>204</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="37">
+        <v>1</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="39"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="35">
+        <v>205</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="39"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+    </row>
+    <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="35">
+        <v>206</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="39"/>
+    </row>
+    <row r="20" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="35">
+        <v>207</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="39"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
+    </row>
+    <row r="21" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="35">
+        <v>208</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="39"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="39"/>
+    </row>
+    <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="35">
+        <v>209</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="37">
         <v>2</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="27">
-        <v>201</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="8">
-        <v>4</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="E22" s="38"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="39"/>
+    </row>
+    <row r="23" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="35">
+        <v>210</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="37">
+        <v>2</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="39"/>
+    </row>
+    <row r="24" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="35">
+        <v>211</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="37">
+        <v>2</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39"/>
+    </row>
+    <row r="25" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="35">
+        <v>212</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="37">
+        <v>2</v>
+      </c>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="39"/>
+    </row>
+    <row r="26" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="35">
+        <v>213</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="37">
+        <v>2</v>
+      </c>
+      <c r="E26" s="38"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="39"/>
+    </row>
+    <row r="27" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="35">
+        <v>214</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="37">
+        <v>2</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="39"/>
+    </row>
+    <row r="28" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="35">
+        <v>215</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="37">
+        <v>2</v>
+      </c>
+      <c r="E28" s="38"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="39"/>
+    </row>
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="21">
+        <v>700</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="27">
-        <v>202</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="8">
-        <v>6</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="33"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="F29" s="22"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="28"/>
+    </row>
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="23">
+        <v>701</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="27">
-        <v>203</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="F30" s="24"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="23">
+        <v>702</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="33"/>
-    </row>
-    <row r="17" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="30">
-        <v>204</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="14">
-        <v>10</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="31"/>
-    </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="F31" s="24"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="23">
+        <v>703</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="29"/>
+    </row>
+    <row r="33" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="26">
+        <v>704</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="25">
-        <v>700</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B34" s="21">
+        <v>801</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="34"/>
-    </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="27">
-        <v>701</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B35" s="23">
+        <v>802</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="35"/>
-    </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="27">
-        <v>702</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="27">
-        <v>703</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="35"/>
-    </row>
-    <row r="22" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="30">
-        <v>704</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="37"/>
-    </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="25">
-        <v>801</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="34"/>
-    </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="27">
-        <v>802</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="35"/>
-    </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="27">
-        <v>803</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="27">
-        <v>804</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="35"/>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="27">
-        <v>805</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="27">
-        <v>806</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="28"/>
-    </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="27">
-        <v>807</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="35"/>
-    </row>
-    <row r="30" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="27">
-        <v>808</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="28"/>
-    </row>
-    <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="27">
-        <v>809</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="28"/>
-    </row>
-    <row r="32" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="30">
-        <v>810</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="36"/>
-    </row>
-    <row r="33" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="38">
-        <v>900</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="29"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="27">
-        <v>901</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="28"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="27">
-        <v>902</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="28"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F35" s="24"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="29"/>
+    </row>
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="27">
-        <v>903</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="23">
+        <v>803</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="28"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F36" s="24"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="29"/>
+    </row>
+    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="27">
-        <v>904</v>
+        <v>37</v>
+      </c>
+      <c r="B37" s="23">
+        <v>804</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="28"/>
-    </row>
-    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="29"/>
+    </row>
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="27">
-        <v>905</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="23">
+        <v>805</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="29"/>
     </row>
     <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="27">
-        <v>906</v>
+        <v>39</v>
+      </c>
+      <c r="B39" s="23">
+        <v>806</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="28"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="24"/>
       <c r="G39" s="3"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="28"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="27">
-        <v>907</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="23">
+        <v>807</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="28" t="s">
+      <c r="F40" s="24"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="29"/>
+    </row>
+    <row r="41" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="23">
+        <v>808</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="23">
+        <v>809</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="26">
+        <v>810</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="30"/>
+    </row>
+    <row r="44" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="32">
+        <v>900</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="25"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="23">
+        <v>901</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="23">
+        <v>902</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="23">
+        <v>903</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="23">
+        <v>904</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="23">
+        <v>905</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F49" s="24"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="24"/>
+    </row>
+    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="23">
+        <v>906</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="24"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="24"/>
+    </row>
+    <row r="51" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="23">
+        <v>907</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="28" t="s">
+      <c r="G51" s="3"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+    <row r="52" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B52" s="26">
         <v>908</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="36" t="s">
+      <c r="D52" s="4"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="36" t="s">
+      <c r="G52" s="4"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="30" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initialized Collection Point Installation Phase
with the "new" concept: one operation_sequence per element
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -14,13 +14,13 @@
   <sheets>
     <sheet name="operations" sheetId="18" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>Mobilisation</t>
   </si>
@@ -368,6 +368,21 @@
   </si>
   <si>
     <t>Connect to guide wire + Lower cable and connection equip + Perform wet-mate connect + Recover connection equip</t>
+  </si>
+  <si>
+    <t>Lift array/export cable-end from seabed</t>
+  </si>
+  <si>
+    <t>LiftCable</t>
+  </si>
+  <si>
+    <t>DryConnect</t>
+  </si>
+  <si>
+    <t>LowerCP</t>
+  </si>
+  <si>
+    <t>Conduct dry-mate connection on deck</t>
   </si>
 </sst>
 </file>
@@ -419,7 +434,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -770,11 +785,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -891,6 +915,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1197,16 +1224,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
@@ -1796,7 +1823,7 @@
       <c r="J27" s="38"/>
       <c r="K27" s="39"/>
     </row>
-    <row r="28" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>111</v>
       </c>
@@ -1817,142 +1844,146 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="35">
+        <v>216</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="40">
+        <v>2</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="39"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="35">
+        <v>217</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="40">
+        <v>2</v>
+      </c>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="35">
+        <v>218</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="40">
+        <v>2</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="39"/>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B32" s="21">
         <v>700</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="11" t="s">
+      <c r="D32" s="14"/>
+      <c r="E32" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="28"/>
-    </row>
-    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="F32" s="22"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="28"/>
+    </row>
+    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B33" s="23">
         <v>701</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="1" t="s">
+      <c r="D33" s="7"/>
+      <c r="E33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="29"/>
-    </row>
-    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="F33" s="24"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B34" s="23">
         <v>702</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="1" t="s">
+      <c r="D34" s="7"/>
+      <c r="E34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="29"/>
-    </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="F34" s="24"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="29"/>
+    </row>
+    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B35" s="23">
         <v>703</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="1" t="s">
+      <c r="D35" s="7"/>
+      <c r="E35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="29"/>
-    </row>
-    <row r="33" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="26">
-        <v>704</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="31"/>
-    </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="21">
-        <v>801</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="28"/>
-    </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="23">
-        <v>802</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="1"/>
       <c r="F35" s="24"/>
       <c r="G35" s="9"/>
       <c r="H35" s="6"/>
@@ -1960,53 +1991,55 @@
       <c r="J35" s="6"/>
       <c r="K35" s="29"/>
     </row>
-    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="23">
-        <v>803</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="29"/>
-    </row>
-    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="23">
-        <v>804</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="29"/>
-    </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="26">
+        <v>704</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="21">
+        <v>801</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="28"/>
+    </row>
+    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B38" s="23">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="1"/>
@@ -2019,32 +2052,32 @@
     </row>
     <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B39" s="23">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="1"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="24"/>
-    </row>
-    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="G39" s="9"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="29"/>
+    </row>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" s="23">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="1"/>
@@ -2055,34 +2088,34 @@
       <c r="J40" s="6"/>
       <c r="K40" s="29"/>
     </row>
-    <row r="41" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41" s="23">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="1"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="24"/>
-    </row>
-    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="9"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="29"/>
+    </row>
+    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B42" s="23">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="1"/>
@@ -2093,53 +2126,53 @@
       <c r="J42" s="1"/>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="26">
-        <v>810</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="30"/>
-    </row>
-    <row r="44" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="32">
-        <v>900</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="25"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="23">
+        <v>807</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="29"/>
+    </row>
+    <row r="44" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="23">
+        <v>808</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="24"/>
+    </row>
+    <row r="45" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B45" s="23">
-        <v>901</v>
+        <v>809</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="1"/>
@@ -2150,56 +2183,56 @@
       <c r="J45" s="1"/>
       <c r="K45" s="24"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="23">
-        <v>902</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="24"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="23">
-        <v>903</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="24"/>
+    <row r="46" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="26">
+        <v>810</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="30"/>
+    </row>
+    <row r="47" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="32">
+        <v>900</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="25"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B48" s="23">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D48" s="3"/>
-      <c r="E48" s="33"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="24"/>
       <c r="G48" s="3"/>
       <c r="H48" s="1"/>
@@ -2207,20 +2240,18 @@
       <c r="J48" s="1"/>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B49" s="23">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="1"/>
       <c r="F49" s="24"/>
       <c r="G49" s="3"/>
       <c r="H49" s="1"/>
@@ -2228,20 +2259,18 @@
       <c r="J49" s="1"/>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B50" s="23">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D50" s="3"/>
-      <c r="E50" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="24"/>
       <c r="G50" s="3"/>
       <c r="H50" s="1"/>
@@ -2249,49 +2278,110 @@
       <c r="J50" s="1"/>
       <c r="K50" s="24"/>
     </row>
-    <row r="51" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B51" s="23">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D51" s="3"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="E51" s="33"/>
+      <c r="F51" s="24"/>
       <c r="G51" s="3"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="24" t="s">
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="23">
+        <v>905</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="24"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="23">
+        <v>906</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="24"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="24"/>
+    </row>
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="23">
+        <v>907</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="G54" s="3"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B55" s="26">
         <v>908</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="30" t="s">
+      <c r="D55" s="4"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="30" t="s">
+      <c r="G55" s="4"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="30" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working Version - EI updated
Collection Point characterized and tested
Dynamic Cable characterized
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
   <si>
     <t>Mobilisation</t>
   </si>
@@ -331,48 +331,15 @@
     <t>H_progressrate</t>
   </si>
   <si>
-    <t>OnTerm_OCT</t>
-  </si>
-  <si>
-    <t>OnTerm_HDD</t>
-  </si>
-  <si>
-    <t>OffTerm_Dev_Con</t>
-  </si>
-  <si>
-    <t>OffTerm_DynCable</t>
-  </si>
-  <si>
-    <t>OffTerm_Dev_Jtube</t>
-  </si>
-  <si>
-    <t>OffTerm_CP_HardW</t>
-  </si>
-  <si>
-    <t>OffTerm_CP_Dry</t>
-  </si>
-  <si>
-    <t>OffTerm_CP_Wet</t>
-  </si>
-  <si>
-    <t>OffTerm_CP_Jtube</t>
-  </si>
-  <si>
     <t>J-tube entrance inspection + Guide wire connection + Cable lay + Cable pull + Cable connection</t>
   </si>
   <si>
-    <t>Lower cable end to the seabed</t>
-  </si>
-  <si>
     <t>Lower collection point to the seabed</t>
   </si>
   <si>
     <t>Connect to guide wire + Lower cable and connection equip + Perform wet-mate connect + Recover connection equip</t>
   </si>
   <si>
-    <t>Lift array/export cable-end from seabed</t>
-  </si>
-  <si>
     <t>LiftCable</t>
   </si>
   <si>
@@ -383,6 +350,54 @@
   </si>
   <si>
     <t>Conduct dry-mate connection on deck</t>
+  </si>
+  <si>
+    <t>Term_Dev_Jtube</t>
+  </si>
+  <si>
+    <t>Term_CP_HardW</t>
+  </si>
+  <si>
+    <t>Term_CP_Wet</t>
+  </si>
+  <si>
+    <t>Term_CP_Jtube</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>Term_Static_Wet</t>
+  </si>
+  <si>
+    <t>Term_Static_Dry</t>
+  </si>
+  <si>
+    <t>Term_Static_Splice</t>
+  </si>
+  <si>
+    <t>LowerCable</t>
+  </si>
+  <si>
+    <t>Lower cable-end from seabed</t>
+  </si>
+  <si>
+    <t>Lift cable-end from seabed</t>
+  </si>
+  <si>
+    <t>Lift cable-end from seabed + Conduct dry-mate connection on deck + lower cable connection to the seabed</t>
+  </si>
+  <si>
+    <t>Lift cable-end from seabed + Conduct splice connection on deck + lower cable connection to the seabed</t>
+  </si>
+  <si>
+    <t>DynCableLay</t>
+  </si>
+  <si>
+    <t>Cable lay with buoyancy modules</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1546,7 @@
     </row>
     <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B14" s="35">
         <v>201</v>
@@ -1552,7 +1567,7 @@
     </row>
     <row r="15" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B15" s="35">
         <v>202</v>
@@ -1613,7 +1628,7 @@
       <c r="J17" s="38"/>
       <c r="K17" s="39"/>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>93</v>
       </c>
@@ -1699,18 +1714,18 @@
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B22" s="35">
         <v>209</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="37">
-        <v>2</v>
-      </c>
-      <c r="E22" s="38"/>
+        <v>125</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="38" t="s">
+        <v>102</v>
+      </c>
       <c r="F22" s="39"/>
       <c r="G22" s="37"/>
       <c r="H22" s="38"/>
@@ -1720,13 +1735,13 @@
     </row>
     <row r="23" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B23" s="35">
         <v>210</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D23" s="37">
         <v>2</v>
@@ -1739,15 +1754,15 @@
       <c r="J23" s="38"/>
       <c r="K23" s="39"/>
     </row>
-    <row r="24" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B24" s="35">
         <v>211</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D24" s="37">
         <v>2</v>
@@ -1760,15 +1775,15 @@
       <c r="J24" s="38"/>
       <c r="K24" s="39"/>
     </row>
-    <row r="25" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B25" s="35">
         <v>212</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D25" s="37">
         <v>2</v>
@@ -1781,15 +1796,15 @@
       <c r="J25" s="38"/>
       <c r="K25" s="39"/>
     </row>
-    <row r="26" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B26" s="35">
         <v>213</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D26" s="37">
         <v>2</v>
@@ -1802,15 +1817,15 @@
       <c r="J26" s="38"/>
       <c r="K26" s="39"/>
     </row>
-    <row r="27" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B27" s="35">
         <v>214</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D27" s="37">
         <v>2</v>
@@ -1823,15 +1838,15 @@
       <c r="J27" s="38"/>
       <c r="K27" s="39"/>
     </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B28" s="35">
         <v>215</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D28" s="37">
         <v>2</v>
@@ -1844,17 +1859,17 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B29" s="35">
         <v>216</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="40">
+        <v>103</v>
+      </c>
+      <c r="D29" s="37">
         <v>2</v>
       </c>
       <c r="E29" s="38"/>
@@ -1865,9 +1880,9 @@
       <c r="J29" s="38"/>
       <c r="K29" s="39"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="35">
         <v>217</v>
@@ -1875,9 +1890,7 @@
       <c r="C30" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="40">
-        <v>2</v>
-      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="38"/>
       <c r="F30" s="39"/>
       <c r="G30" s="37"/>
@@ -1886,15 +1899,15 @@
       <c r="J30" s="38"/>
       <c r="K30" s="39"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B31" s="35">
         <v>218</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D31" s="40">
         <v>2</v>
@@ -1907,82 +1920,82 @@
       <c r="J31" s="38"/>
       <c r="K31" s="39"/>
     </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="35">
+        <v>219</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="40">
+        <v>2</v>
+      </c>
+      <c r="E32" s="38"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="39"/>
+    </row>
+    <row r="33" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="35">
+        <v>220</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="40">
+        <v>2</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="39"/>
+    </row>
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="21">
+      <c r="B34" s="21">
         <v>700</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="11" t="s">
+      <c r="D34" s="14"/>
+      <c r="E34" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="28"/>
-    </row>
-    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="F34" s="22"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B35" s="23">
         <v>701</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="29"/>
-    </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="23">
-        <v>702</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="29"/>
-    </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="23">
-        <v>703</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="9"/>
@@ -1991,93 +2004,97 @@
       <c r="J35" s="6"/>
       <c r="K35" s="29"/>
     </row>
-    <row r="36" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="23">
+        <v>702</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="24"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="29"/>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="23">
+        <v>703</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="24"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="29"/>
+    </row>
+    <row r="38" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B38" s="26">
         <v>704</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="2" t="s">
+      <c r="D38" s="17"/>
+      <c r="E38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="31"/>
-    </row>
-    <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="F38" s="30"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B39" s="21">
         <v>801</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="28"/>
-    </row>
-    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="28"/>
+    </row>
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B40" s="23">
         <v>802</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="29"/>
-    </row>
-    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="23">
-        <v>803</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="29"/>
-    </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="23">
-        <v>804</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="1"/>
@@ -2088,15 +2105,15 @@
       <c r="J40" s="6"/>
       <c r="K40" s="29"/>
     </row>
-    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B41" s="23">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="1"/>
@@ -2107,34 +2124,34 @@
       <c r="J41" s="6"/>
       <c r="K41" s="29"/>
     </row>
-    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" s="23">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="1"/>
       <c r="F42" s="24"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="24"/>
-    </row>
-    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="G42" s="9"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="29"/>
+    </row>
+    <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B43" s="23">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="1"/>
@@ -2145,15 +2162,15 @@
       <c r="J43" s="6"/>
       <c r="K43" s="29"/>
     </row>
-    <row r="44" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B44" s="23">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="1"/>
@@ -2164,110 +2181,110 @@
       <c r="J44" s="1"/>
       <c r="K44" s="24"/>
     </row>
-    <row r="45" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B45" s="23">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="1"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="24"/>
-    </row>
-    <row r="46" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="29"/>
+    </row>
+    <row r="46" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="23">
+        <v>808</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="23">
+        <v>809</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B48" s="26">
         <v>810</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="30"/>
-    </row>
-    <row r="47" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="D48" s="4"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="30"/>
+    </row>
+    <row r="49" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="32">
+      <c r="B49" s="32">
         <v>900</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="25"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="23">
-        <v>901</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="24"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="23">
-        <v>902</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="24"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="25"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B50" s="23">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="1"/>
@@ -2280,16 +2297,16 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" s="23">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D51" s="3"/>
-      <c r="E51" s="33"/>
+      <c r="E51" s="1"/>
       <c r="F51" s="24"/>
       <c r="G51" s="3"/>
       <c r="H51" s="1"/>
@@ -2297,20 +2314,18 @@
       <c r="J51" s="1"/>
       <c r="K51" s="24"/>
     </row>
-    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B52" s="23">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="24"/>
       <c r="G52" s="3"/>
       <c r="H52" s="1"/>
@@ -2318,20 +2333,18 @@
       <c r="J52" s="1"/>
       <c r="K52" s="24"/>
     </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B53" s="23">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="E53" s="33"/>
       <c r="F53" s="24"/>
       <c r="G53" s="3"/>
       <c r="H53" s="1"/>
@@ -2339,49 +2352,91 @@
       <c r="J53" s="1"/>
       <c r="K53" s="24"/>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B54" s="23">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="24" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="24"/>
       <c r="G54" s="3"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="24" t="s">
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="23">
+        <v>906</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" s="24"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="23">
+        <v>907</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="G56" s="3"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="26">
+      <c r="B57" s="26">
         <v>908</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="30" t="s">
+      <c r="D57" s="4"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G55" s="4"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="30" t="s">
+      <c r="G57" s="4"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="30" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mostly some cleaning to prepare schedule.py
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteillant\Documents\DTOcean-WP5\src\databases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="264" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="264"/>
   </bookViews>
   <sheets>
-    <sheet name="operations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="operations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
   <si>
     <t>id [-]</t>
   </si>
@@ -53,9 +57,6 @@
     <t>Mobilisation</t>
   </si>
   <si>
-    <t>vesselsDB("Mob time [h]")</t>
-  </si>
-  <si>
     <t>AssPort</t>
   </si>
   <si>
@@ -74,16 +75,10 @@
     <t>Transportation from port to site</t>
   </si>
   <si>
-    <t>transit distance algorithm(port, site) * vessel transit speed</t>
-  </si>
-  <si>
     <t>TranSitePort</t>
   </si>
   <si>
-    <t>Transportation from site to port </t>
-  </si>
-  <si>
-    <t>transit distance algorithm(site, port) * vessel transit speed</t>
+    <t>Transportation from site to port</t>
   </si>
   <si>
     <t>TranSiteSite</t>
@@ -92,18 +87,12 @@
     <t>Transportation from site to site</t>
   </si>
   <si>
-    <t>transit distance algorithm(site, site) * vessel transit speed</t>
-  </si>
-  <si>
     <t>Demob</t>
   </si>
   <si>
     <t>Demobilisation</t>
   </si>
   <si>
-    <t>vesselDB("Mob time [h]")</t>
-  </si>
-  <si>
     <t>SeafloorEquipPrep</t>
   </si>
   <si>
@@ -113,7 +102,7 @@
     <t>Grout</t>
   </si>
   <si>
-    <t>Grouting </t>
+    <t>Grouting</t>
   </si>
   <si>
     <t>average grouting rate*volume of grouting</t>
@@ -122,7 +111,7 @@
     <t>GroutRemov</t>
   </si>
   <si>
-    <t>Grouting equipment removal </t>
+    <t>Grouting equipment removal</t>
   </si>
   <si>
     <t>SuppStrutPos</t>
@@ -170,9 +159,6 @@
     <t>Cable lay and burial through cable route</t>
   </si>
   <si>
-    <t>H_progressrate</t>
-  </si>
-  <si>
     <t>CableLayRoute</t>
   </si>
   <si>
@@ -260,45 +246,30 @@
     <t>Driven pile foundation or anchor seafloor penetration through drilling rig + positioning</t>
   </si>
   <si>
-    <t>penetration depth * vertical penetration rate(drilling, soil type)</t>
-  </si>
-  <si>
     <t>PileHamm</t>
   </si>
   <si>
     <t>Driven pile foundation or anchor seafloor penetration through hammering + positioning</t>
   </si>
   <si>
-    <t>penetration depth * vertical penetration rate(hammering, soil type)</t>
-  </si>
-  <si>
     <t>PileVibro</t>
   </si>
   <si>
     <t>Driven pile foundation or anchor seafloor penetration through vibro-driving + positioning</t>
   </si>
   <si>
-    <t>penetration depth * vertical penetration rate(vibro-driving, soil type)</t>
-  </si>
-  <si>
     <t>GBSpos</t>
   </si>
   <si>
     <t>Gravity based foundation or anchor lowering + positioning</t>
   </si>
   <si>
-    <t>water depth * (60% *max lowering rate)</t>
-  </si>
-  <si>
     <t>SuctCais</t>
   </si>
   <si>
     <t>Suction caisson foundation or anchor seafloor penetration + positioning</t>
   </si>
   <si>
-    <t>penetration depth *  vertical penetration rate(suction pump, soil type)</t>
-  </si>
-  <si>
     <t>DragEmbed</t>
   </si>
   <si>
@@ -341,9 +312,6 @@
     <t>Device assembly at port</t>
   </si>
   <si>
-    <t>user_inputs['device']['assembly duration [h]']</t>
-  </si>
-  <si>
     <t>LoadOut_Lift</t>
   </si>
   <si>
@@ -374,18 +342,12 @@
     <t>Deck transportation</t>
   </si>
   <si>
-    <t>transit distance algorithm(port, site)  * vessel transit speed</t>
-  </si>
-  <si>
     <t>TowTrans</t>
   </si>
   <si>
     <t>Towing transportation</t>
   </si>
   <si>
-    <t>transit distance algorithm(port, site) * vessel towing speed</t>
-  </si>
-  <si>
     <t>PosBFdev</t>
   </si>
   <si>
@@ -399,65 +361,77 @@
   </si>
   <si>
     <t>On-site posisitioning and connection of floating device</t>
+  </si>
+  <si>
+    <t>transit_algorithm(UTM_i, UTM_f) * vesselDB['vessel transit speed']</t>
+  </si>
+  <si>
+    <t>distance(UTM_i, UTM_f) * vesselDB['vessel transit speed']</t>
+  </si>
+  <si>
+    <t>vesselsDB['Mob time [h]']</t>
+  </si>
+  <si>
+    <t>penetration_time</t>
+  </si>
+  <si>
+    <t>laying_time</t>
+  </si>
+  <si>
+    <t>device['assembly duration [h]']</t>
+  </si>
+  <si>
+    <t>transit_algorithm(UTM_i, UTM_f)  * vesselDB['vessel transit speed']</t>
+  </si>
+  <si>
+    <t>device['connect duration [h]']</t>
+  </si>
+  <si>
+    <t>device['disconnect duration [h]']</t>
+  </si>
+  <si>
+    <t>site['water depth [m]'] * 0.6 *max_lowering_rate(Mass, Dimensions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -469,382 +443,794 @@
     </fill>
   </fills>
   <borders count="27">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thick"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="medium"/>
-      <top style="thick"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thick"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thick"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="medium"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thick"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thick"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="medium"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thick"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="14" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="15" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="16" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="16" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="14" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="17" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="18" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="19" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="20" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="21" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="13" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="22" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="23" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="24" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="25" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="26" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E18" activeCellId="0" pane="topLeft" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.678431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4862745098039"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6352941176471"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
+    <col min="1" max="1" width="22"/>
+    <col min="2" max="2" width="8.5703125"/>
+    <col min="3" max="3" width="38.140625"/>
+    <col min="4" max="4" width="21.42578125"/>
+    <col min="5" max="5" width="24.5703125"/>
+    <col min="6" max="6" width="25.7109375"/>
+    <col min="7" max="7" width="14.42578125"/>
+    <col min="8" max="8" width="14.85546875"/>
+    <col min="9" max="9" width="16.85546875"/>
+    <col min="10" max="10" width="16.5703125"/>
+    <col min="11" max="11" width="16.42578125"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="37.5" outlineLevel="0" r="1">
+    <row r="1" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -877,11 +1263,11 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3">
         <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -890,7 +1276,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="2"/>
@@ -898,17 +1284,17 @@
       <c r="J2" s="2"/>
       <c r="K2" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="3">
+    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7">
+        <v>101</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>101</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3" s="6"/>
@@ -919,17 +1305,17 @@
       <c r="J3" s="6"/>
       <c r="K3" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="4">
+    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7">
+        <v>102</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>102</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="8">
         <v>48</v>
       </c>
       <c r="E4" s="6"/>
@@ -940,19 +1326,19 @@
       <c r="J4" s="6"/>
       <c r="K4" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="5">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7">
+        <v>103</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>103</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8"/>
@@ -961,19 +1347,19 @@
       <c r="J5" s="6"/>
       <c r="K5" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="6">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7">
         <v>104</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
@@ -982,19 +1368,19 @@
       <c r="J6" s="6"/>
       <c r="K6" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="7">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7">
         <v>105</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -1003,20 +1389,20 @@
       <c r="J7" s="6"/>
       <c r="K7" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="7" t="n">
+        <v>22</v>
+      </c>
+      <c r="B8" s="7">
         <v>106</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>116</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="6"/>
@@ -1024,17 +1410,17 @@
       <c r="J8" s="6"/>
       <c r="K8" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" s="7">
         <v>107</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" s="8">
         <v>1</v>
       </c>
       <c r="E9" s="6"/>
@@ -1045,19 +1431,19 @@
       <c r="J9" s="6"/>
       <c r="K9" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7">
         <v>108</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="8"/>
@@ -1066,17 +1452,17 @@
       <c r="J10" s="6"/>
       <c r="K10" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="22.5" outlineLevel="0" r="11">
+    <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="7" t="n">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7">
         <v>109</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8">
         <v>0.5</v>
       </c>
       <c r="E11" s="6"/>
@@ -1087,17 +1473,17 @@
       <c r="J11" s="6"/>
       <c r="K11" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="B12" s="11">
         <v>110</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="D12" s="13">
         <v>2</v>
       </c>
       <c r="E12" s="14"/>
@@ -1108,19 +1494,19 @@
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="17" t="n">
+        <v>33</v>
+      </c>
+      <c r="B13" s="17">
         <v>200</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="19"/>
@@ -1129,17 +1515,17 @@
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="52.5" outlineLevel="0" r="14">
+    <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="17" t="n">
+        <v>36</v>
+      </c>
+      <c r="B14" s="17">
         <v>201</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="19" t="n">
+        <v>37</v>
+      </c>
+      <c r="D14" s="19">
         <v>10</v>
       </c>
       <c r="E14" s="20"/>
@@ -1150,17 +1536,17 @@
       <c r="J14" s="20"/>
       <c r="K14" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="51.75" outlineLevel="0" r="15">
+    <row r="15" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="17" t="n">
+        <v>38</v>
+      </c>
+      <c r="B15" s="17">
         <v>202</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="19" t="n">
+        <v>39</v>
+      </c>
+      <c r="D15" s="19">
         <v>10</v>
       </c>
       <c r="E15" s="20"/>
@@ -1171,17 +1557,17 @@
       <c r="J15" s="20"/>
       <c r="K15" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.25" outlineLevel="0" r="16">
+    <row r="16" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="17" t="n">
+        <v>40</v>
+      </c>
+      <c r="B16" s="17">
         <v>203</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="19" t="n">
+        <v>41</v>
+      </c>
+      <c r="D16" s="19">
         <v>1</v>
       </c>
       <c r="E16" s="20"/>
@@ -1192,17 +1578,17 @@
       <c r="J16" s="20"/>
       <c r="K16" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.25" outlineLevel="0" r="17">
+    <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="17" t="n">
+        <v>42</v>
+      </c>
+      <c r="B17" s="17">
         <v>204</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="19" t="n">
+        <v>43</v>
+      </c>
+      <c r="D17" s="19">
         <v>1</v>
       </c>
       <c r="E17" s="20"/>
@@ -1213,19 +1599,19 @@
       <c r="J17" s="20"/>
       <c r="K17" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="17" t="n">
+        <v>44</v>
+      </c>
+      <c r="B18" s="17">
         <v>205</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="19"/>
@@ -1234,19 +1620,19 @@
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.75" outlineLevel="0" r="19">
+    <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="17" t="n">
+        <v>46</v>
+      </c>
+      <c r="B19" s="17">
         <v>206</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="20" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="19"/>
@@ -1255,19 +1641,19 @@
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.75" outlineLevel="0" r="20">
+    <row r="20" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="17" t="n">
+        <v>48</v>
+      </c>
+      <c r="B20" s="17">
         <v>207</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="19"/>
@@ -1276,19 +1662,19 @@
       <c r="J20" s="20"/>
       <c r="K20" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.75" outlineLevel="0" r="21">
+    <row r="21" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="B21" s="17">
         <v>208</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="19"/>
@@ -1297,19 +1683,19 @@
       <c r="J21" s="20"/>
       <c r="K21" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.75" outlineLevel="0" r="22">
+    <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="17" t="n">
+        <v>52</v>
+      </c>
+      <c r="B22" s="17">
         <v>209</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="20" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="19"/>
@@ -1318,17 +1704,17 @@
       <c r="J22" s="20"/>
       <c r="K22" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="23">
+    <row r="23" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="17" t="n">
+        <v>54</v>
+      </c>
+      <c r="B23" s="17">
         <v>210</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="19" t="n">
+        <v>55</v>
+      </c>
+      <c r="D23" s="19">
         <v>2</v>
       </c>
       <c r="E23" s="20"/>
@@ -1339,17 +1725,17 @@
       <c r="J23" s="20"/>
       <c r="K23" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54.75" outlineLevel="0" r="24">
+    <row r="24" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="17" t="n">
+        <v>56</v>
+      </c>
+      <c r="B24" s="17">
         <v>211</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="19" t="n">
+        <v>57</v>
+      </c>
+      <c r="D24" s="19">
         <v>2</v>
       </c>
       <c r="E24" s="20"/>
@@ -1360,17 +1746,17 @@
       <c r="J24" s="20"/>
       <c r="K24" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="52.5" outlineLevel="0" r="25">
+    <row r="25" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="17" t="n">
+        <v>58</v>
+      </c>
+      <c r="B25" s="17">
         <v>212</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="19" t="n">
+        <v>59</v>
+      </c>
+      <c r="D25" s="19">
         <v>2</v>
       </c>
       <c r="E25" s="20"/>
@@ -1381,17 +1767,17 @@
       <c r="J25" s="20"/>
       <c r="K25" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="50.25" outlineLevel="0" r="26">
+    <row r="26" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B26" s="17">
         <v>213</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="19" t="n">
+        <v>61</v>
+      </c>
+      <c r="D26" s="19">
         <v>2</v>
       </c>
       <c r="E26" s="20"/>
@@ -1402,17 +1788,17 @@
       <c r="J26" s="20"/>
       <c r="K26" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.75" outlineLevel="0" r="27">
+    <row r="27" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="17" t="n">
+        <v>62</v>
+      </c>
+      <c r="B27" s="17">
         <v>214</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="19" t="n">
+        <v>63</v>
+      </c>
+      <c r="D27" s="19">
         <v>2</v>
       </c>
       <c r="E27" s="20"/>
@@ -1423,17 +1809,17 @@
       <c r="J27" s="20"/>
       <c r="K27" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.25" outlineLevel="0" r="28">
+    <row r="28" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="17" t="n">
+        <v>64</v>
+      </c>
+      <c r="B28" s="17">
         <v>215</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="19" t="n">
+        <v>57</v>
+      </c>
+      <c r="D28" s="19">
         <v>2</v>
       </c>
       <c r="E28" s="20"/>
@@ -1444,17 +1830,17 @@
       <c r="J28" s="20"/>
       <c r="K28" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="29">
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="17" t="n">
+        <v>65</v>
+      </c>
+      <c r="B29" s="17">
         <v>216</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="19" t="n">
+        <v>55</v>
+      </c>
+      <c r="D29" s="19">
         <v>2</v>
       </c>
       <c r="E29" s="20"/>
@@ -1465,15 +1851,15 @@
       <c r="J29" s="20"/>
       <c r="K29" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="22.5" outlineLevel="0" r="30">
+    <row r="30" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="17" t="n">
+        <v>66</v>
+      </c>
+      <c r="B30" s="17">
         <v>217</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="20"/>
@@ -1484,17 +1870,17 @@
       <c r="J30" s="20"/>
       <c r="K30" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="31">
+    <row r="31" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="17" t="n">
+        <v>68</v>
+      </c>
+      <c r="B31" s="17">
         <v>218</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="22" t="n">
+        <v>69</v>
+      </c>
+      <c r="D31" s="22">
         <v>2</v>
       </c>
       <c r="E31" s="20"/>
@@ -1505,17 +1891,17 @@
       <c r="J31" s="20"/>
       <c r="K31" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.25" outlineLevel="0" r="32">
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="17" t="n">
+        <v>70</v>
+      </c>
+      <c r="B32" s="17">
         <v>219</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="22" t="n">
+        <v>71</v>
+      </c>
+      <c r="D32" s="22">
         <v>2</v>
       </c>
       <c r="E32" s="20"/>
@@ -1526,17 +1912,17 @@
       <c r="J32" s="20"/>
       <c r="K32" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.75" outlineLevel="0" r="33">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="17" t="n">
+        <v>72</v>
+      </c>
+      <c r="B33" s="17">
         <v>220</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="22" t="n">
+        <v>63</v>
+      </c>
+      <c r="D33" s="22">
         <v>2</v>
       </c>
       <c r="E33" s="20"/>
@@ -1547,19 +1933,19 @@
       <c r="J33" s="20"/>
       <c r="K33" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="34">
+    <row r="34" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B34" s="3">
         <v>700</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="2" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="24"/>
@@ -1568,19 +1954,19 @@
       <c r="J34" s="25"/>
       <c r="K34" s="26"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="35">
+    <row r="35" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="B35" s="7">
         <v>701</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D35" s="27"/>
-      <c r="E35" s="6" t="s">
-        <v>84</v>
+      <c r="E35" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="28"/>
@@ -1589,19 +1975,19 @@
       <c r="J35" s="29"/>
       <c r="K35" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="36">
+    <row r="36" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="7" t="n">
+        <v>77</v>
+      </c>
+      <c r="B36" s="7">
         <v>702</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D36" s="27"/>
-      <c r="E36" s="6" t="s">
-        <v>87</v>
+      <c r="E36" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="28"/>
@@ -1610,19 +1996,19 @@
       <c r="J36" s="29"/>
       <c r="K36" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="37">
+    <row r="37" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="7" t="n">
+        <v>79</v>
+      </c>
+      <c r="B37" s="7">
         <v>703</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="6" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="28"/>
@@ -1631,19 +2017,19 @@
       <c r="J37" s="29"/>
       <c r="K37" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="38">
+    <row r="38" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="11" t="n">
+        <v>81</v>
+      </c>
+      <c r="B38" s="11">
         <v>704</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D38" s="31"/>
-      <c r="E38" s="10" t="s">
-        <v>93</v>
+      <c r="E38" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F38" s="32"/>
       <c r="G38" s="33"/>
@@ -1652,15 +2038,15 @@
       <c r="J38" s="34"/>
       <c r="K38" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="39">
+    <row r="39" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B39" s="3">
         <v>801</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="2"/>
@@ -1671,15 +2057,15 @@
       <c r="J39" s="25"/>
       <c r="K39" s="26"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="40">
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="B40" s="7">
         <v>802</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="6"/>
@@ -1690,15 +2076,15 @@
       <c r="J40" s="29"/>
       <c r="K40" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="41">
+    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="7" t="n">
+        <v>77</v>
+      </c>
+      <c r="B41" s="7">
         <v>803</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="6"/>
@@ -1709,15 +2095,15 @@
       <c r="J41" s="29"/>
       <c r="K41" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="42">
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="7" t="n">
+        <v>79</v>
+      </c>
+      <c r="B42" s="7">
         <v>804</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="6"/>
@@ -1728,15 +2114,15 @@
       <c r="J42" s="29"/>
       <c r="K42" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.6" outlineLevel="0" r="43">
+    <row r="43" spans="1:11" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="7" t="n">
+        <v>83</v>
+      </c>
+      <c r="B43" s="7">
         <v>805</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="6"/>
@@ -1747,15 +2133,15 @@
       <c r="J43" s="29"/>
       <c r="K43" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="44">
+    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="B44" s="7">
         <v>806</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="6"/>
@@ -1766,15 +2152,15 @@
       <c r="J44" s="6"/>
       <c r="K44" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="45">
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="7" t="n">
+        <v>87</v>
+      </c>
+      <c r="B45" s="7">
         <v>807</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="6"/>
@@ -1785,15 +2171,15 @@
       <c r="J45" s="29"/>
       <c r="K45" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54.75" outlineLevel="0" r="46">
+    <row r="46" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="7" t="n">
+        <v>89</v>
+      </c>
+      <c r="B46" s="7">
         <v>808</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="6"/>
@@ -1804,15 +2190,15 @@
       <c r="J46" s="6"/>
       <c r="K46" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="27" outlineLevel="0" r="47">
+    <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="7" t="n">
+        <v>91</v>
+      </c>
+      <c r="B47" s="7">
         <v>809</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="6"/>
@@ -1823,15 +2209,15 @@
       <c r="J47" s="6"/>
       <c r="K47" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33" outlineLevel="0" r="48">
+    <row r="48" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="11" t="n">
+        <v>93</v>
+      </c>
+      <c r="B48" s="11">
         <v>810</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="10"/>
@@ -1842,20 +2228,20 @@
       <c r="J48" s="10"/>
       <c r="K48" s="32"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="34.5" outlineLevel="0" r="49">
+    <row r="49" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" s="37" t="n">
+        <v>95</v>
+      </c>
+      <c r="B49" s="37">
         <v>900</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D49" s="38"/>
       <c r="E49" s="36"/>
       <c r="F49" s="39" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G49" s="38"/>
       <c r="H49" s="36"/>
@@ -1863,15 +2249,15 @@
       <c r="J49" s="36"/>
       <c r="K49" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="50">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="7" t="n">
+        <v>97</v>
+      </c>
+      <c r="B50" s="7">
         <v>901</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="6"/>
@@ -1882,15 +2268,15 @@
       <c r="J50" s="6"/>
       <c r="K50" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="51">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="7" t="n">
+        <v>99</v>
+      </c>
+      <c r="B51" s="7">
         <v>902</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="6"/>
@@ -1901,15 +2287,15 @@
       <c r="J51" s="6"/>
       <c r="K51" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="52">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="7" t="n">
+        <v>101</v>
+      </c>
+      <c r="B52" s="7">
         <v>903</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="6"/>
@@ -1920,15 +2306,15 @@
       <c r="J52" s="6"/>
       <c r="K52" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="53">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" s="7" t="n">
+        <v>103</v>
+      </c>
+      <c r="B53" s="7">
         <v>904</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="40"/>
@@ -1939,19 +2325,19 @@
       <c r="J53" s="6"/>
       <c r="K53" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="54">
+    <row r="54" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="7" t="n">
+        <v>105</v>
+      </c>
+      <c r="B54" s="7">
         <v>905</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="8"/>
@@ -1960,19 +2346,19 @@
       <c r="J54" s="6"/>
       <c r="K54" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="55">
+    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55" s="7" t="n">
+        <v>107</v>
+      </c>
+      <c r="B55" s="7">
         <v>906</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="8"/>
@@ -1981,59 +2367,54 @@
       <c r="J55" s="6"/>
       <c r="K55" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="56">
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" s="7" t="n">
+        <v>109</v>
+      </c>
+      <c r="B56" s="7">
         <v>907</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="6"/>
       <c r="F56" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="57">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="11" t="n">
+        <v>112</v>
+      </c>
+      <c r="B57" s="11">
         <v>908</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="10"/>
       <c r="F57" s="32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="32" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
engage with time assessment of the onshore activities
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
   <si>
     <t>id [-]</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Grouting</t>
   </si>
   <si>
-    <t>average grouting rate*volume of grouting</t>
-  </si>
-  <si>
     <t>GroutRemov</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Loading cable from factory port</t>
   </si>
   <si>
-    <t>loadcable</t>
-  </si>
-  <si>
     <t>OCT</t>
   </si>
   <si>
@@ -363,12 +357,6 @@
     <t>On-site posisitioning and connection of floating device</t>
   </si>
   <si>
-    <t>transit_algorithm(UTM_i, UTM_f) * vesselDB['vessel transit speed']</t>
-  </si>
-  <si>
-    <t>distance(UTM_i, UTM_f) * vesselDB['vessel transit speed']</t>
-  </si>
-  <si>
     <t>vesselsDB['Mob time [h]']</t>
   </si>
   <si>
@@ -381,16 +369,25 @@
     <t>device['assembly duration [h]']</t>
   </si>
   <si>
-    <t>transit_algorithm(UTM_i, UTM_f)  * vesselDB['vessel transit speed']</t>
-  </si>
-  <si>
     <t>device['connect duration [h]']</t>
   </si>
   <si>
     <t>device['disconnect duration [h]']</t>
   </si>
   <si>
-    <t>site['water depth [m]'] * 0.6 *max_lowering_rate(Mass, Dimensions)</t>
+    <t>transit_algorithm</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>grouting</t>
+  </si>
+  <si>
+    <t>load_cable</t>
+  </si>
+  <si>
+    <t>lowering</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1273,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="2"/>
@@ -1326,7 +1323,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1338,7 +1335,7 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8"/>
@@ -1347,7 +1344,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1359,7 +1356,7 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
@@ -1368,7 +1365,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -1380,7 +1377,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="8"/>
@@ -1402,7 +1399,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="6"/>
@@ -1431,7 +1428,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1443,7 +1440,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="8"/>
@@ -1454,13 +1451,13 @@
     </row>
     <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7">
         <v>109</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="8">
         <v>0.5</v>
@@ -1475,13 +1472,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="11">
         <v>110</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="13">
         <v>2</v>
@@ -1496,17 +1493,17 @@
     </row>
     <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="17">
         <v>200</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="19"/>
@@ -1517,13 +1514,13 @@
     </row>
     <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="17">
         <v>201</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="19">
         <v>10</v>
@@ -1538,13 +1535,13 @@
     </row>
     <row r="15" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="17">
         <v>202</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="19">
         <v>10</v>
@@ -1559,13 +1556,13 @@
     </row>
     <row r="16" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="17">
         <v>203</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -1580,13 +1577,13 @@
     </row>
     <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="17">
         <v>204</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -1601,17 +1598,17 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="17">
         <v>205</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="19"/>
@@ -1622,17 +1619,17 @@
     </row>
     <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="17">
         <v>206</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="19"/>
@@ -1643,17 +1640,17 @@
     </row>
     <row r="20" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="17">
         <v>207</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="19"/>
@@ -1664,17 +1661,17 @@
     </row>
     <row r="21" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="17">
         <v>208</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="19"/>
@@ -1685,17 +1682,17 @@
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="17">
         <v>209</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="19"/>
@@ -1706,13 +1703,13 @@
     </row>
     <row r="23" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" s="17">
         <v>210</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="19">
         <v>2</v>
@@ -1727,13 +1724,13 @@
     </row>
     <row r="24" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="17">
         <v>211</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="19">
         <v>2</v>
@@ -1748,13 +1745,13 @@
     </row>
     <row r="25" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="17">
         <v>212</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="19">
         <v>2</v>
@@ -1769,13 +1766,13 @@
     </row>
     <row r="26" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="17">
         <v>213</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="19">
         <v>2</v>
@@ -1790,13 +1787,13 @@
     </row>
     <row r="27" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="17">
         <v>214</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="19">
         <v>2</v>
@@ -1811,13 +1808,13 @@
     </row>
     <row r="28" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="17">
         <v>215</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="19">
         <v>2</v>
@@ -1832,13 +1829,13 @@
     </row>
     <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="17">
         <v>216</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="19">
         <v>2</v>
@@ -1853,13 +1850,13 @@
     </row>
     <row r="30" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="17">
         <v>217</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="20"/>
@@ -1872,13 +1869,13 @@
     </row>
     <row r="31" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" s="17">
         <v>218</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" s="22">
         <v>2</v>
@@ -1893,13 +1890,13 @@
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="17">
         <v>219</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D32" s="22">
         <v>2</v>
@@ -1914,13 +1911,13 @@
     </row>
     <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="17">
         <v>220</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33" s="22">
         <v>2</v>
@@ -1935,17 +1932,17 @@
     </row>
     <row r="34" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3">
         <v>700</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="24"/>
@@ -1956,17 +1953,17 @@
     </row>
     <row r="35" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B35" s="7">
         <v>701</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="27"/>
       <c r="E35" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="28"/>
@@ -1977,17 +1974,17 @@
     </row>
     <row r="36" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B36" s="7">
         <v>702</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D36" s="27"/>
       <c r="E36" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="28"/>
@@ -1996,19 +1993,19 @@
       <c r="J36" s="29"/>
       <c r="K36" s="30"/>
     </row>
-    <row r="37" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" s="7">
         <v>703</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="28"/>
@@ -2019,17 +2016,17 @@
     </row>
     <row r="38" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B38" s="11">
         <v>704</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" s="31"/>
       <c r="E38" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F38" s="32"/>
       <c r="G38" s="33"/>
@@ -2040,16 +2037,18 @@
     </row>
     <row r="39" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="3">
         <v>801</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F39" s="5"/>
       <c r="G39" s="24"/>
       <c r="H39" s="25"/>
@@ -2057,18 +2056,20 @@
       <c r="J39" s="25"/>
       <c r="K39" s="26"/>
     </row>
-    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" s="7">
         <v>802</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="8"/>
-      <c r="E40" s="6"/>
+      <c r="E40" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F40" s="9"/>
       <c r="G40" s="28"/>
       <c r="H40" s="29"/>
@@ -2076,18 +2077,20 @@
       <c r="J40" s="29"/>
       <c r="K40" s="30"/>
     </row>
-    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" s="7">
         <v>803</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="6"/>
+      <c r="E41" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F41" s="9"/>
       <c r="G41" s="28"/>
       <c r="H41" s="29"/>
@@ -2095,18 +2098,20 @@
       <c r="J41" s="29"/>
       <c r="K41" s="30"/>
     </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B42" s="7">
         <v>804</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="8"/>
-      <c r="E42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="28"/>
       <c r="H42" s="29"/>
@@ -2114,17 +2119,19 @@
       <c r="J42" s="29"/>
       <c r="K42" s="30"/>
     </row>
-    <row r="43" spans="1:11" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="28.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B43" s="7">
         <v>805</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E43" s="6"/>
       <c r="F43" s="9"/>
       <c r="G43" s="28"/>
@@ -2133,18 +2140,20 @@
       <c r="J43" s="29"/>
       <c r="K43" s="30"/>
     </row>
-    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" s="7">
         <v>806</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D44" s="8"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F44" s="9"/>
       <c r="G44" s="8"/>
       <c r="H44" s="6"/>
@@ -2152,18 +2161,20 @@
       <c r="J44" s="6"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B45" s="7">
         <v>807</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" s="8"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F45" s="9"/>
       <c r="G45" s="28"/>
       <c r="H45" s="29"/>
@@ -2171,18 +2182,20 @@
       <c r="J45" s="29"/>
       <c r="K45" s="30"/>
     </row>
-    <row r="46" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="54.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B46" s="7">
         <v>808</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D46" s="8"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F46" s="9"/>
       <c r="G46" s="8"/>
       <c r="H46" s="6"/>
@@ -2190,17 +2203,19 @@
       <c r="J46" s="6"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B47" s="7">
         <v>809</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E47" s="6"/>
       <c r="F47" s="9"/>
       <c r="G47" s="8"/>
@@ -2211,15 +2226,17 @@
     </row>
     <row r="48" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="11">
         <v>810</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="D48" s="12">
+        <v>0.5</v>
+      </c>
       <c r="E48" s="10"/>
       <c r="F48" s="32"/>
       <c r="G48" s="12"/>
@@ -2230,18 +2247,18 @@
     </row>
     <row r="49" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" s="37">
         <v>900</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D49" s="38"/>
       <c r="E49" s="36"/>
       <c r="F49" s="39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G49" s="38"/>
       <c r="H49" s="36"/>
@@ -2251,15 +2268,17 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B50" s="7">
         <v>901</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="D50" s="8">
+        <v>1</v>
+      </c>
       <c r="E50" s="6"/>
       <c r="F50" s="9"/>
       <c r="G50" s="8"/>
@@ -2270,15 +2289,17 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B51" s="7">
         <v>902</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="D51" s="8">
+        <v>2</v>
+      </c>
       <c r="E51" s="6"/>
       <c r="F51" s="9"/>
       <c r="G51" s="8"/>
@@ -2289,15 +2310,17 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B52" s="7">
         <v>903</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D52" s="8"/>
+        <v>100</v>
+      </c>
+      <c r="D52" s="8">
+        <v>4</v>
+      </c>
       <c r="E52" s="6"/>
       <c r="F52" s="9"/>
       <c r="G52" s="8"/>
@@ -2308,15 +2331,17 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B53" s="7">
         <v>904</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E53" s="40"/>
       <c r="F53" s="9"/>
       <c r="G53" s="8"/>
@@ -2325,19 +2350,19 @@
       <c r="J53" s="6"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="7">
         <v>905</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="8"/>
@@ -2346,19 +2371,19 @@
       <c r="J54" s="6"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="7">
         <v>906</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="8"/>
@@ -2369,48 +2394,48 @@
     </row>
     <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B56" s="7">
         <v>907</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="6"/>
       <c r="F56" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="11">
         <v>908</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="10"/>
       <c r="F57" s="32" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logistic phase characterization and DB update
Vessel DB has been post-processed
Collection Point has been characterized (corrected)
Gravity Structures has been characterized (corrected)
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteillant\Documents\DTOcean-WP5\src\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchainho\Documents\DTOcean-WP5-Installation\src\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="264"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="264"/>
   </bookViews>
   <sheets>
     <sheet name="operations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
   <si>
     <t>id [-]</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>lowering</t>
+  </si>
+  <si>
+    <t>JUP jacking time</t>
+  </si>
+  <si>
+    <t>GBSlower</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,11 +2009,13 @@
       <c r="C37" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F37" s="9"/>
+      <c r="D37" s="27">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="G37" s="28"/>
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
@@ -2100,7 +2108,7 @@
     </row>
     <row r="42" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="B42" s="7">
         <v>804</v>

</xml_diff>

<commit_message>
getting there for a simplified schedule_device
</commit_message>
<xml_diff>
--- a/src/databases/operations_time_OLC.xlsx
+++ b/src/databases/operations_time_OLC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchainho\Documents\DTOcean-WP5-Installation\src\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteillant\Documents\DTOcean-WP5\src\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="149">
   <si>
     <t>id [-]</t>
   </si>
@@ -348,9 +348,6 @@
     <t>device['connect duration [h]']</t>
   </si>
   <si>
-    <t>device['disconnect duration [h]']</t>
-  </si>
-  <si>
     <t>transit_algorithm</t>
   </si>
   <si>
@@ -454,6 +451,21 @@
   </si>
   <si>
     <t>Inspection or Maintenance Operations</t>
+  </si>
+  <si>
+    <t>vessel</t>
+  </si>
+  <si>
+    <t>device['max Hs [m]']</t>
+  </si>
+  <si>
+    <t>device['max Tp [s]']</t>
+  </si>
+  <si>
+    <t>device['max Ws [m/s]']</t>
+  </si>
+  <si>
+    <t>device['max Cs [m/s]']</t>
   </si>
 </sst>
 </file>
@@ -505,7 +517,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -980,19 +992,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1029,7 +1028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1223,19 +1222,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1524,10 +1520,10 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I59" sqref="I59"/>
+      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,13 +1650,21 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="G5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1675,13 +1679,21 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="G6" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,13 +1708,21 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="G7" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1741,10 +1761,18 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="G9" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,13 +1787,21 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="G10" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1783,34 +1819,50 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="G11" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="62">
         <v>110</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="64">
         <v>1</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="66"/>
+        <v>114</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="K12" s="65"/>
     </row>
     <row r="13" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
@@ -1827,10 +1879,18 @@
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
+      <c r="G13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K13" s="48"/>
     </row>
     <row r="14" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1845,7 +1905,7 @@
       </c>
       <c r="D14" s="49"/>
       <c r="E14" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="51"/>
@@ -2274,13 +2334,13 @@
     </row>
     <row r="35" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="39">
         <v>300</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="53">
         <v>2</v>
@@ -2295,13 +2355,13 @@
     </row>
     <row r="36" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" s="20">
         <v>301</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
@@ -2392,7 +2452,7 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="4"/>
@@ -2402,7 +2462,7 @@
     </row>
     <row r="41" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="21">
         <v>306</v>
@@ -2412,7 +2472,7 @@
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="57"/>
@@ -2429,7 +2489,7 @@
         <v>400</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D42" s="41">
         <v>1.5</v>
@@ -2444,13 +2504,13 @@
     </row>
     <row r="43" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="20">
         <v>401</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" s="1">
         <v>1.5</v>
@@ -2465,13 +2525,13 @@
     </row>
     <row r="44" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="20">
         <v>402</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -2494,7 +2554,7 @@
         <v>403</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -2517,7 +2577,7 @@
         <v>404</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -2540,7 +2600,7 @@
         <v>405</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -2693,13 +2753,21 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F54" s="11"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
+      <c r="G54" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K54" s="6"/>
     </row>
     <row r="55" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2714,13 +2782,21 @@
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F55" s="11"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
+      <c r="G55" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K55" s="6"/>
     </row>
     <row r="56" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2738,10 +2814,18 @@
       <c r="F56" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
+      <c r="G56" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="K56" s="6" t="s">
         <v>101</v>
       </c>
@@ -2758,67 +2842,75 @@
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="F57" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
+      <c r="F57" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="K57" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="68" t="s">
+      <c r="A58" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="66">
+        <v>600</v>
+      </c>
+      <c r="C58" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="67">
-        <v>600</v>
-      </c>
-      <c r="C58" s="69" t="s">
+      <c r="F58" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="F58" s="70" t="s">
+      <c r="G58" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="H58" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="I58" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="J58" s="69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="66">
+        <v>601</v>
+      </c>
+      <c r="C59" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="G58" s="70" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="70" t="s">
-        <v>135</v>
-      </c>
-      <c r="I58" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="J58" s="70" t="s">
+      <c r="G59" s="69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="68" t="s">
-        <v>143</v>
-      </c>
-      <c r="B59" s="67">
-        <v>601</v>
-      </c>
-      <c r="C59" s="69" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="G59" s="70" t="s">
+      <c r="H59" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="H59" s="70" t="s">
+      <c r="I59" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="I59" s="70" t="s">
+      <c r="J59" s="69" t="s">
         <v>140</v>
-      </c>
-      <c r="J59" s="70" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>